<commit_message>
Renamed Investor to Stakeholder in CDP and KYC files
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distribution_payments.xlsx
+++ b/public/sample_uploads/capital_distribution_payments.xlsx
@@ -222,7 +222,7 @@
     <t xml:space="preserve">Fund *</t>
   </si>
   <si>
-    <t xml:space="preserve">Investor *</t>
+    <t xml:space="preserve">Stakeholder *</t>
   </si>
   <si>
     <t xml:space="preserve">Capital Distribution *</t>
@@ -417,31 +417,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -641,7 +641,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G7"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>